<commit_message>
updated runtime and fixed errors
</commit_message>
<xml_diff>
--- a/Warehouses.xlsx
+++ b/Warehouses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugogiao\OneDrive - VG\Ambiente de Trabalho\blockly-spaces\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugoa\Desktop\classes2021\Dissertation\spreadsheet_processes\blockly-spaces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF2588F-648B-4C6F-B55F-CDE8E8ABEA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B815C64D-F49E-45FC-A6DA-A235A6AFCFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3275EF75-58B7-476D-B030-7D95D6146BE8}"/>
+    <workbookView xWindow="975" yWindow="300" windowWidth="14145" windowHeight="10620" xr2:uid="{3275EF75-58B7-476D-B030-7D95D6146BE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,43 +30,43 @@
     <t>Warehouses</t>
   </si>
   <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>Sigma</t>
+  </si>
+  <si>
+    <t>Warehouse1_shipping</t>
+  </si>
+  <si>
+    <t>Warehouse2_shipping</t>
+  </si>
+  <si>
     <t>Warehouse1</t>
   </si>
   <si>
     <t>Warehouse2</t>
-  </si>
-  <si>
-    <t>Customer1</t>
-  </si>
-  <si>
-    <t>Empty</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Customers</t>
-  </si>
-  <si>
-    <t>Customer2</t>
-  </si>
-  <si>
-    <t>Customer3</t>
-  </si>
-  <si>
-    <t>Customer4</t>
-  </si>
-  <si>
-    <t>Warehouse1_shipping</t>
-  </si>
-  <si>
-    <t>Warehouse2_shipping</t>
-  </si>
-  <si>
-    <t>Orders</t>
-  </si>
-  <si>
-    <t>Available</t>
   </si>
 </sst>
 </file>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -421,22 +421,22 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" customWidth="1"/>
-    <col min="2" max="2" width="22.26953125" customWidth="1"/>
-    <col min="3" max="3" width="23.453125" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -445,21 +445,21 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -471,18 +471,18 @@
         <v>35000</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>60000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -494,18 +494,18 @@
         <v>22000</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="G3">
         <v>80000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0.5</v>
@@ -517,10 +517,10 @@
         <v>18000</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -534,7 +534,7 @@
         <v>30000</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>